<commit_message>
DTD - creating and utilizing generic methods
</commit_message>
<xml_diff>
--- a/testdata/customer_data.xlsx
+++ b/testdata/customer_data.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\eclipse\Automation\testdata\"/>
     </mc:Choice>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="23">
   <si>
     <t>SlNo</t>
   </si>
@@ -80,12 +80,22 @@
   </si>
   <si>
     <t>Alok Patel</t>
+  </si>
+  <si>
+    <t>Rahul das</t>
+  </si>
+  <si>
+    <t>Rahul Das</t>
+  </si>
+  <si>
+    <t>Anjana Singh</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -434,10 +444,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="4.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="4.77734375"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="14.33203125"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="30.0"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="9.88671875"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
@@ -455,86 +465,86 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2">
+      <c r="A2" s="0">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" t="s" s="0">
         <v>4</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" t="s" s="0">
         <v>5</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" t="s" s="0">
         <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3">
+      <c r="A3" s="0">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C3" t="s">
+      <c r="B3" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="C3" t="s" s="0">
         <v>7</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" t="s" s="0">
         <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4">
+      <c r="A4" s="0">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" t="s" s="0">
         <v>9</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" t="s" s="0">
         <v>10</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" t="s" s="0">
         <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5">
+      <c r="A5" s="0">
         <v>4</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" t="s" s="0">
         <v>12</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" t="s" s="0">
         <v>13</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" t="s" s="0">
         <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6">
+      <c r="A6" s="0">
         <v>5</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" t="s" s="0">
         <v>14</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" t="s" s="0">
         <v>15</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" t="s" s="0">
         <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7">
+      <c r="A7" s="0">
         <v>6</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" t="s" s="0">
         <v>17</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" t="s" s="0">
         <v>18</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" t="s" s="0">
         <v>8</v>
       </c>
     </row>

</xml_diff>